<commit_message>
More Graphs, Bug Fix Subgroup Termination Graph
</commit_message>
<xml_diff>
--- a/Data/All_Groups_Disease.xlsx
+++ b/Data/All_Groups_Disease.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7550EB70-55AA-431E-94FF-42A37E6CC775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1717C774-C274-4A24-B0AD-7F099E0837C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="11184" yWindow="4932" windowWidth="16692" windowHeight="9228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>group</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Stroke</t>
+  </si>
+  <si>
+    <t>Disease</t>
   </si>
 </sst>
 </file>
@@ -734,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,6 +749,9 @@
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>